<commit_message>
updated with Ngan's reviews
</commit_message>
<xml_diff>
--- a/data/ODHF_mismatches.xlsx
+++ b/data/ODHF_mismatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kt/Documents/UBC_MDS/capstone/data-599-capstone-statistics-canada/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6798EA3-52D4-8D42-BD3F-79A260934C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8469683-F667-2142-9909-CFA588A34388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B248889A-8E44-664A-B39D-7E2FBB35CA0C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
   <si>
     <t>N</t>
   </si>
@@ -66,18 +66,9 @@
     <t>r√àsidence saint-louis</t>
   </si>
   <si>
-    <t>sant√© manitouwadge health</t>
-  </si>
-  <si>
-    <t>st. joseph's health care, london - mount hope centre for long term care - marian villa</t>
-  </si>
-  <si>
     <t>st. joseph's health centre, guelph</t>
   </si>
   <si>
-    <t>st. joseph's mother house (martha wing)</t>
-  </si>
-  <si>
     <t>strathcona long term care</t>
   </si>
   <si>
@@ -156,12 +147,6 @@
     <t>North West</t>
   </si>
   <si>
-    <t>200 College Avenue P.O. Box 5777</t>
-  </si>
-  <si>
-    <t>London, N6A1Y1</t>
-  </si>
-  <si>
     <t>100 Westmount Road</t>
   </si>
   <si>
@@ -171,12 +156,6 @@
     <t>Waterloo Wellington</t>
   </si>
   <si>
-    <t>574 Northcliffe Avenue</t>
-  </si>
-  <si>
-    <t>Dundas, L9H7L9</t>
-  </si>
-  <si>
     <t>465 Dublin Street</t>
   </si>
   <si>
@@ -279,21 +258,94 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>Scraped homes not in ODHF (after cross-referencing)</t>
-  </si>
-  <si>
     <t>Scraped homes not in ODHF (before cross-referencing)</t>
   </si>
   <si>
-    <t>Found in ODHF (Y/N)</t>
+    <t>Mismatch in ODHF (Y/N)</t>
+  </si>
+  <si>
+    <t>ODHF Reference</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>listed in ODHF but no geodata, https://www.peoplecare.ca/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Seems to be attached to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Windsor Regional Hospital</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which is in ODHF if we need the geolocation data. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hotel-dieu grace healthcare css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> has same location in ODHF.</t>
+    </r>
+  </si>
+  <si>
+    <t>seems to be attached to manitouwadge general hospital</t>
+  </si>
+  <si>
+    <t>sante manitouwadge health</t>
+  </si>
+  <si>
+    <t>https://svch.ca/long-term-care/strathcona/location/, in ODHF have saugeen valley nursing center which is at the same address, https://svch.ca/saugeen-valley-nursing-centre-announces-plan-to-redevelop-87-bed-facility-in-mount-forest/#.Xr2rvRNKjfY</t>
+  </si>
+  <si>
+    <t>Scraped homes with mismatch in ODHF (after cross-referencing)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -331,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -434,11 +486,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -456,13 +543,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,342 +886,368 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA17B9DB-B11A-8040-B33E-865295EF0146}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="72.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" thickBot="1">
+    <row r="1" spans="1:6" ht="22" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" ht="34">
+        <v>73</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="34">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B2" s="5">
-        <f>COUNTA(A6:A29)</f>
+        <f>COUNTA(A6:A27)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="52" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="6">
+        <f>COUNTIF(A:A, "Y")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="50" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1" thickBot="1">
+      <c r="A5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" hidden="1" thickTop="1">
+      <c r="A13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" thickTop="1">
+      <c r="A14" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="50" customHeight="1" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="6">
-        <f>COUNTIF(A:A, "N")</f>
+    <row r="15" spans="1:6" hidden="1">
+      <c r="A15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="102">
+      <c r="A16" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1">
+      <c r="A17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1">
+      <c r="A18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1">
+      <c r="A19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1">
+      <c r="A20" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="50" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A5" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34">
+      <c r="A21" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A6" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A9" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A10" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A12" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" hidden="1" thickTop="1">
-      <c r="A13" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" thickTop="1">
-      <c r="A14" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" hidden="1">
-      <c r="A17" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1">
-      <c r="A18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1">
-      <c r="A19" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E21" t="s">
         <v>32</v>
       </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" hidden="1">
-      <c r="A20" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="F21" t="s">
         <v>33</v>
       </c>
-      <c r="D20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" hidden="1">
+    </row>
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B22" s="14"/>
       <c r="C22" t="s">
         <v>9</v>
       </c>
@@ -1124,128 +1257,112 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="51">
+      <c r="A23" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1">
+      <c r="A24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" t="s">
         <v>10</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" t="s">
         <v>37</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E24" t="s">
         <v>38</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:6" ht="170">
+      <c r="A25" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
         <v>40</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E25" t="s">
         <v>41</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1">
+      <c r="A26" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1">
+      <c r="A27" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1">
-      <c r="A25" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" hidden="1">
-      <c r="A28" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" hidden="1">
-      <c r="A29" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" t="s">
-        <v>39</v>
-      </c>
+    <row r="28" spans="1:6">
+      <c r="B28" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:E29" xr:uid="{2F60157F-5D40-C145-9781-6C9D385289BF}">
+  <autoFilter ref="A5:F27" xr:uid="{2F60157F-5D40-C145-9781-6C9D385289BF}">
     <filterColumn colId="0">
       <filters>
-        <filter val="N"/>
+        <filter val="Y"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>